<commit_message>
Billy feuille de temps
</commit_message>
<xml_diff>
--- a/Documents/Documents sprint/Feuille_de_temps.xlsx
+++ b/Documents/Documents sprint/Feuille_de_temps.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\AWT\NovaGo\Documents\Documents sprint\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lechu\Documents\GitHub\NovaGo\Documents\Documents sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321FD912-AB6D-4B43-A063-A67E0312FAB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF5B4F1-8339-4948-A68D-1A950E79CF31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="0" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8745" yWindow="3540" windowWidth="19140" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="70">
   <si>
     <t>Nom</t>
   </si>
@@ -230,6 +230,27 @@
   <si>
     <t>Mise à jour des scripts et du README</t>
   </si>
+  <si>
+    <t>readme</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>server + exploration.ejs</t>
+  </si>
+  <si>
+    <t>plus de 10</t>
+  </si>
+  <si>
+    <t>server + connexion.ejs</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>bootstrap + css</t>
+  </si>
 </sst>
 </file>
 
@@ -335,7 +356,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -381,6 +402,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,7 +423,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -704,7 +728,7 @@
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -897,15 +921,16 @@
   </sheetPr>
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="36.140625" customWidth="1"/>
     <col min="4" max="4" width="26.7109375" customWidth="1"/>
     <col min="6" max="6" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -959,8 +984,12 @@
       <c r="F2" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+      <c r="G2" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>64</v>
+      </c>
       <c r="I2" s="15"/>
       <c r="J2" s="15"/>
     </row>
@@ -983,8 +1012,12 @@
       <c r="F3" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
+      <c r="G3" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="H3" s="19" t="s">
+        <v>66</v>
+      </c>
       <c r="I3" s="15"/>
       <c r="J3" s="15"/>
     </row>
@@ -1003,8 +1036,12 @@
       <c r="F4" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
+      <c r="G4" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" s="15">
+        <v>4</v>
+      </c>
       <c r="I4" s="15"/>
       <c r="J4" s="15"/>
     </row>
@@ -1019,8 +1056,12 @@
       <c r="F5" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="G5" s="15"/>
-      <c r="H5" s="15"/>
+      <c r="G5" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>68</v>
+      </c>
       <c r="I5" s="15"/>
       <c r="J5" s="15"/>
     </row>
@@ -1035,8 +1076,12 @@
       <c r="F6" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
+      <c r="G6" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="H6" s="15" t="s">
+        <v>64</v>
+      </c>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
     </row>
@@ -1168,13 +1213,14 @@
   </sheetPr>
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="8" max="8" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
@@ -1309,7 +1355,7 @@
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -8450,7 +8496,7 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>

</xml_diff>

<commit_message>
update feuille de temps
</commit_message>
<xml_diff>
--- a/Documents/Documents sprint/Feuille_de_temps.xlsx
+++ b/Documents/Documents sprint/Feuille_de_temps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lechu\Documents\GitHub\NovaGo\Documents\Documents sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E53D09D-CB5F-4AD4-B3BD-78977E4A399D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11201690-C34F-4109-BC40-557B1F5DA3C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8745" yWindow="3540" windowWidth="19140" windowHeight="11835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="78">
   <si>
     <t>Nom</t>
   </si>
@@ -268,6 +268,12 @@
   </si>
   <si>
     <t>erreur de base de données (affichage)</t>
+  </si>
+  <si>
+    <t>refaire reservation.ejs</t>
+  </si>
+  <si>
+    <t>~15</t>
   </si>
 </sst>
 </file>
@@ -740,7 +746,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -783,11 +789,11 @@
       <c r="D3" s="6">
         <v>8.5</v>
       </c>
-      <c r="E3" s="6">
-        <v>0</v>
+      <c r="E3" s="6" t="s">
+        <v>77</v>
       </c>
       <c r="F3" s="7">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
@@ -937,7 +943,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1114,8 +1120,12 @@
       <c r="H6" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
+      <c r="I6" s="15">
+        <v>4</v>
+      </c>
+      <c r="J6" s="15" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15"/>
@@ -1246,7 +1256,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4:J4"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Début de l'implémentation de sessions
</commit_message>
<xml_diff>
--- a/Documents/Documents sprint/Feuille_de_temps.xlsx
+++ b/Documents/Documents sprint/Feuille_de_temps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\2034730\Documents\GitHub\NovaGo\Documents\Documents sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3ABDD2-1292-427C-B3BA-3517C7CD4D7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785998A4-9BD8-417C-AB95-53CFF464E3E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="84">
   <si>
     <t>Nom</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>Gestion des documents de sprint</t>
+  </si>
+  <si>
+    <t>Implémentation de validation de session</t>
   </si>
 </sst>
 </file>
@@ -767,7 +770,7 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -1485,8 +1488,8 @@
   </sheetPr>
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1672,8 +1675,12 @@
       <c r="H6" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="I6" s="17"/>
-      <c r="J6" s="14"/>
+      <c r="I6" s="17">
+        <v>1</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="7" spans="1:14" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15"/>

</xml_diff>

<commit_message>
Commentaires et lisibilité dans plusieurs .ejs
</commit_message>
<xml_diff>
--- a/Documents/Documents sprint/Feuille_de_temps.xlsx
+++ b/Documents/Documents sprint/Feuille_de_temps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\2034730\Documents\GitHub\NovaGo\Documents\Documents sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{785998A4-9BD8-417C-AB95-53CFF464E3E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA5006A-95B7-4D5D-BB1F-70285E34DB63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="85">
   <si>
     <t>Nom</t>
   </si>
@@ -292,6 +292,9 @@
   </si>
   <si>
     <t>Implémentation de validation de session</t>
+  </si>
+  <si>
+    <t>Modifications ejs pour standardiser le développement</t>
   </si>
 </sst>
 </file>
@@ -770,8 +773,8 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -868,7 +871,7 @@
         <v>10.5</v>
       </c>
       <c r="F5" s="7">
-        <v>4</v>
+        <v>7.5</v>
       </c>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
@@ -937,7 +940,7 @@
         <v>7</v>
       </c>
       <c r="E10" s="9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
@@ -957,7 +960,7 @@
         <v>7</v>
       </c>
       <c r="E11" s="6">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
@@ -976,7 +979,9 @@
       <c r="D12" s="9">
         <v>4</v>
       </c>
-      <c r="E12" s="9"/>
+      <c r="E12" s="9">
+        <v>6</v>
+      </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
@@ -1488,8 +1493,8 @@
   </sheetPr>
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1563,12 +1568,16 @@
       <c r="H2" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="15">
         <v>2.5</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="15" t="s">
         <v>68</v>
       </c>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
     </row>
     <row r="3" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="14">
@@ -1595,12 +1604,16 @@
       <c r="H3" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="15">
         <v>0.5</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="15" t="s">
         <v>69</v>
       </c>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15"/>
+      <c r="N3" s="15"/>
     </row>
     <row r="4" spans="1:14" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A4" s="17">
@@ -1629,6 +1642,10 @@
       <c r="J4" s="14" t="s">
         <v>78</v>
       </c>
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
     </row>
     <row r="5" spans="1:14" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="17">
@@ -1657,6 +1674,10 @@
       <c r="J5" s="14" t="s">
         <v>82</v>
       </c>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
     </row>
     <row r="6" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17">
@@ -1676,13 +1697,17 @@
         <v>58</v>
       </c>
       <c r="I6" s="17">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="J6" s="14" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+    </row>
+    <row r="7" spans="1:14" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15"/>
       <c r="B7" s="14"/>
       <c r="C7" s="15"/>
@@ -1695,8 +1720,16 @@
       <c r="H7" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="I7" s="15"/>
-      <c r="J7" s="14"/>
+      <c r="I7" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="12"/>

</xml_diff>

<commit_message>
Index liste planètes v1
</commit_message>
<xml_diff>
--- a/Documents/Documents sprint/Feuille_de_temps.xlsx
+++ b/Documents/Documents sprint/Feuille_de_temps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\NovaGo\Documents\Documents sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C760AA5D-E6F0-427B-B478-016C225FF674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD00DAF-22E8-4FC1-9D52-6AA5824CCB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="96">
   <si>
     <t>Nom</t>
   </si>
@@ -325,6 +325,9 @@
   </si>
   <si>
     <t>Commentaires/ petits fix</t>
+  </si>
+  <si>
+    <t>Affichage de la liste de planetes dans index</t>
   </si>
 </sst>
 </file>
@@ -803,7 +806,7 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -908,7 +911,7 @@
         <v>9</v>
       </c>
       <c r="G5" s="7">
-        <v>4</v>
+        <v>6.5</v>
       </c>
       <c r="H5" s="7"/>
     </row>
@@ -1573,7 +1576,7 @@
   </sheetPr>
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
@@ -1798,8 +1801,12 @@
       <c r="J6" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="K6" s="17"/>
-      <c r="L6" s="17"/>
+      <c r="K6" s="17">
+        <v>2</v>
+      </c>
+      <c r="L6" s="17" t="s">
+        <v>95</v>
+      </c>
       <c r="M6" s="17"/>
       <c r="N6" s="17"/>
     </row>

</xml_diff>

<commit_message>
Index liste planètes v2
</commit_message>
<xml_diff>
--- a/Documents/Documents sprint/Feuille_de_temps.xlsx
+++ b/Documents/Documents sprint/Feuille_de_temps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\NovaGo\Documents\Documents sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AD00DAF-22E8-4FC1-9D52-6AA5824CCB89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A61A256-0B4C-487B-B6F4-894C373F96A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -806,8 +806,8 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -911,7 +911,7 @@
         <v>9</v>
       </c>
       <c r="G5" s="7">
-        <v>6.5</v>
+        <v>7</v>
       </c>
       <c r="H5" s="7"/>
     </row>
@@ -1010,7 +1010,9 @@
       <c r="F11" s="7">
         <v>6</v>
       </c>
-      <c r="G11" s="7"/>
+      <c r="G11" s="7">
+        <v>6</v>
+      </c>
       <c r="H11" s="7"/>
     </row>
     <row r="12" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
@@ -1576,8 +1578,8 @@
   </sheetPr>
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1802,7 +1804,7 @@
         <v>82</v>
       </c>
       <c r="K6" s="17">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="L6" s="17" t="s">
         <v>95</v>

</xml_diff>

<commit_message>
Début fix bouton Chercher un voyage
</commit_message>
<xml_diff>
--- a/Documents/Documents sprint/Feuille_de_temps.xlsx
+++ b/Documents/Documents sprint/Feuille_de_temps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\NovaGo\Documents\Documents sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B91EE01-F169-4CBF-B78E-92C1CE88D1B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D97D4B-2A03-4EE7-8205-05A3540D3D95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="104">
   <si>
     <t>Nom</t>
   </si>
@@ -349,6 +349,9 @@
   </si>
   <si>
     <t>Affichage des pages sans paramètre mtn possible</t>
+  </si>
+  <si>
+    <t>Fix bouton Chercher un voyage de la page Exploration</t>
   </si>
 </sst>
 </file>
@@ -1632,7 +1635,7 @@
   <dimension ref="A1:N1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1878,8 +1881,12 @@
       <c r="L6" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="M6" s="17"/>
-      <c r="N6" s="17"/>
+      <c r="M6" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="N6" s="17" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="7" spans="1:14" ht="50.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15"/>

</xml_diff>

<commit_message>
Fix est_connecte page inscription
</commit_message>
<xml_diff>
--- a/Documents/Documents sprint/Feuille_de_temps.xlsx
+++ b/Documents/Documents sprint/Feuille_de_temps.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\AWT\NovaGo\Documents\Documents sprint\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\2034730\Documents\GitHub\NovaGo\Documents\Documents sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BD12BEC-EA93-4E30-B193-A3F526A796CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51AA6332-351D-460D-A3AD-5AE28DFEA172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -562,7 +562,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -863,11 +863,11 @@
   </sheetPr>
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -975,7 +975,7 @@
         <v>9.5</v>
       </c>
       <c r="H5" s="7">
-        <v>9</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -1117,11 +1117,11 @@
   </sheetPr>
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="36.140625" customWidth="1"/>
     <col min="4" max="4" width="26.7109375" customWidth="1"/>
@@ -1463,7 +1463,7 @@
       <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
     <col min="8" max="8" width="33.7109375" customWidth="1"/>
@@ -1720,10 +1720,10 @@
   <dimension ref="A1:N1000"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1891,7 +1891,7 @@
         <v>93</v>
       </c>
       <c r="M4" s="17">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="N4" s="17" t="s">
         <v>100</v>
@@ -8984,7 +8984,7 @@
       <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>

</xml_diff>

<commit_message>
Affichage simplifié des messages aux utilisateurs
</commit_message>
<xml_diff>
--- a/Documents/Documents sprint/Feuille_de_temps.xlsx
+++ b/Documents/Documents sprint/Feuille_de_temps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\2034730\Documents\GitHub\NovaGo\Documents\Documents sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51AA6332-351D-460D-A3AD-5AE28DFEA172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DD59AF7-1E52-4EBC-9409-DCDD8C5C0D92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="116">
   <si>
     <t>Nom</t>
   </si>
@@ -385,6 +385,9 @@
   </si>
   <si>
     <t>Implémentation des comptes admins</t>
+  </si>
+  <si>
+    <t>bouttons Boostrap</t>
   </si>
 </sst>
 </file>
@@ -864,7 +867,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -920,10 +923,10 @@
         <v>14</v>
       </c>
       <c r="G3" s="7">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H3" s="7">
-        <v>0.5</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -949,7 +952,7 @@
         <v>8</v>
       </c>
       <c r="H4" s="10">
-        <v>0.5</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.25">
@@ -1001,7 +1004,7 @@
         <v>4</v>
       </c>
       <c r="H6" s="10">
-        <v>0.5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1118,7 +1121,7 @@
   <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1208,10 +1211,10 @@
         <v>68</v>
       </c>
       <c r="K2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L2" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="M2" s="17">
         <v>0.5</v>
@@ -1255,7 +1258,13 @@
         <v>4</v>
       </c>
       <c r="L3" t="s">
-        <v>108</v>
+        <v>106</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1285,11 +1294,11 @@
       <c r="J4" t="s">
         <v>72</v>
       </c>
-      <c r="K4">
-        <v>2</v>
-      </c>
-      <c r="L4" t="s">
-        <v>107</v>
+      <c r="M4">
+        <v>4</v>
+      </c>
+      <c r="N4" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1314,6 +1323,12 @@
       </c>
       <c r="J5" s="15" t="s">
         <v>71</v>
+      </c>
+      <c r="M5">
+        <v>3</v>
+      </c>
+      <c r="N5" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1460,7 +1475,7 @@
   <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fix merge feuille de temps
</commit_message>
<xml_diff>
--- a/Documents/Documents sprint/Feuille_de_temps.xlsx
+++ b/Documents/Documents sprint/Feuille_de_temps.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lechu\Documents\GitHub\NovaGo\Documents\Documents sprint\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\2034730\Documents\GitHub\NovaGo\Documents\Documents sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D95806A-7841-49E4-920B-1EF414CDF02B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C86F2ED-5F29-47F1-AC91-8A27232B226C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="129">
   <si>
     <t>Nom</t>
   </si>
@@ -399,9 +399,6 @@
     <t>Correction logique try catch</t>
   </si>
   <si>
-    <t>Regex client side inscription</t>
-  </si>
-  <si>
     <t>Globalisation des propriétés de session</t>
   </si>
   <si>
@@ -424,6 +421,12 @@
   </si>
   <si>
     <t>nombres d'argents total (js)</t>
+  </si>
+  <si>
+    <t>Regex client side inscription, connexion</t>
+  </si>
+  <si>
+    <t>Testing injection SQL</t>
   </si>
 </sst>
 </file>
@@ -902,8 +905,8 @@
   </sheetPr>
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1019,7 +1022,7 @@
         <v>19</v>
       </c>
       <c r="H5" s="7">
-        <v>5</v>
+        <v>5.5</v>
       </c>
       <c r="I5" s="7"/>
     </row>
@@ -1270,7 +1273,7 @@
         <v>2.5</v>
       </c>
       <c r="N2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1354,7 +1357,7 @@
         <v>1</v>
       </c>
       <c r="N4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1390,7 +1393,7 @@
         <v>1</v>
       </c>
       <c r="N5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1426,7 +1429,7 @@
         <v>1</v>
       </c>
       <c r="N6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1452,7 +1455,7 @@
         <v>1</v>
       </c>
       <c r="N7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1702,7 +1705,7 @@
         <v>1</v>
       </c>
       <c r="N3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1742,7 +1745,7 @@
         <v>0.5</v>
       </c>
       <c r="N4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1770,7 +1773,7 @@
         <v>2</v>
       </c>
       <c r="N5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1852,8 +1855,8 @@
   </sheetPr>
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2073,7 +2076,7 @@
         <v>2.5</v>
       </c>
       <c r="N5" s="17" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
       <c r="O5" s="17"/>
       <c r="P5" s="17"/>
@@ -2106,6 +2109,12 @@
       </c>
       <c r="L6" s="17" t="s">
         <v>95</v>
+      </c>
+      <c r="M6" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="N6" s="17" t="s">
+        <v>128</v>
       </c>
       <c r="O6" s="17"/>
       <c r="P6" s="17"/>

</xml_diff>

<commit_message>
modif feuille de temps
</commit_message>
<xml_diff>
--- a/Documents/Documents sprint/Feuille_de_temps.xlsx
+++ b/Documents/Documents sprint/Feuille_de_temps.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\2034730\Documents\GitHub\NovaGo\Documents\Documents sprint\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lechu\Documents\GitHub\NovaGo\Documents\Documents sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D513EA66-8A6F-4EB9-B59D-C29697A22307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9027C14-B435-4D7E-9CF0-BF45797CFC97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="134">
   <si>
     <t>Nom</t>
   </si>
@@ -436,6 +436,12 @@
   </si>
   <si>
     <t>AJAX inscription</t>
+  </si>
+  <si>
+    <t>css + modifier ejs html pour info voyage</t>
+  </si>
+  <si>
+    <t>server.js pour info voyage (recevoir les données de planet et vaisseau</t>
   </si>
 </sst>
 </file>
@@ -1181,8 +1187,8 @@
   </sheetPr>
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1480,6 +1486,12 @@
       </c>
       <c r="I8" s="15"/>
       <c r="J8" s="15"/>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15"/>
@@ -1490,6 +1502,12 @@
       <c r="F9" s="15"/>
       <c r="I9" s="15"/>
       <c r="J9" s="15"/>
+      <c r="M9">
+        <v>3</v>
+      </c>
+      <c r="N9" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15"/>
@@ -1864,8 +1882,8 @@
   </sheetPr>
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Utilisation d'AJAX lors de déconnexion
</commit_message>
<xml_diff>
--- a/Documents/Documents sprint/Feuille_de_temps.xlsx
+++ b/Documents/Documents sprint/Feuille_de_temps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\NovaGo\Documents\Documents sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8915EF6E-2A19-4804-A0EB-5EBB6643F687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E12E54-BE1F-4EE4-8DAE-F5F7993D3A9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="137">
   <si>
     <t>Nom</t>
   </si>
@@ -448,6 +448,9 @@
   </si>
   <si>
     <t>Session planete</t>
+  </si>
+  <si>
+    <t>AJAX deconnexion</t>
   </si>
 </sst>
 </file>
@@ -926,7 +929,7 @@
   </sheetPr>
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -1043,7 +1046,7 @@
         <v>19</v>
       </c>
       <c r="H5" s="7">
-        <v>7.5</v>
+        <v>9.5</v>
       </c>
       <c r="I5" s="7"/>
     </row>
@@ -1901,11 +1904,14 @@
   </sheetPr>
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="14" max="14" width="15.453125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -2274,6 +2280,12 @@
       </c>
       <c r="L11" s="17" t="s">
         <v>102</v>
+      </c>
+      <c r="M11" s="17">
+        <v>2</v>
+      </c>
+      <c r="N11" s="17" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fix connexion au compte admin
</commit_message>
<xml_diff>
--- a/Documents/Documents sprint/Feuille_de_temps.xlsx
+++ b/Documents/Documents sprint/Feuille_de_temps.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\AWT\NovaGo\Documents\Documents sprint\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\2034730\Documents\GitHub\NovaGo\Documents\Documents sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D95ABCA-A840-4040-BB28-69F73E5AE2D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27DA751B-866A-4524-9519-166CC0E9BCB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="138">
   <si>
     <t>Nom</t>
   </si>
@@ -451,6 +451,9 @@
   </si>
   <si>
     <t>Correction d'erreurs dans le Word</t>
+  </si>
+  <si>
+    <t>AJAX déconnexion</t>
   </si>
 </sst>
 </file>
@@ -628,7 +631,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -929,11 +932,11 @@
   </sheetPr>
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -992,7 +995,7 @@
         <v>15.5</v>
       </c>
       <c r="H3" s="7">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="I3" s="7"/>
     </row>
@@ -1019,7 +1022,7 @@
         <v>16.5</v>
       </c>
       <c r="H4" s="10">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="I4" s="10"/>
     </row>
@@ -1046,7 +1049,7 @@
         <v>19</v>
       </c>
       <c r="H5" s="7">
-        <v>6.5</v>
+        <v>9.5</v>
       </c>
       <c r="I5" s="7"/>
     </row>
@@ -1072,7 +1075,9 @@
       <c r="G6" s="10">
         <v>6</v>
       </c>
-      <c r="H6" s="10"/>
+      <c r="H6" s="10">
+        <v>3</v>
+      </c>
       <c r="I6" s="10"/>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1200,7 +1205,7 @@
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="36.140625" customWidth="1"/>
     <col min="4" max="4" width="26.7109375" customWidth="1"/>
@@ -1599,11 +1604,11 @@
   </sheetPr>
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
     <col min="8" max="8" width="33.7109375" customWidth="1"/>
@@ -1905,10 +1910,10 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -2247,7 +2252,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="12"/>
       <c r="D10" s="12"/>
       <c r="F10" s="12"/>
@@ -2258,6 +2263,12 @@
       </c>
       <c r="L10" s="17" t="s">
         <v>100</v>
+      </c>
+      <c r="M10" s="17">
+        <v>2</v>
+      </c>
+      <c r="N10" s="17" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -9228,10 +9239,10 @@
   <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>

</xml_diff>

<commit_message>
Début envoie session à la BD
</commit_message>
<xml_diff>
--- a/Documents/Documents sprint/Feuille_de_temps.xlsx
+++ b/Documents/Documents sprint/Feuille_de_temps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\2034730\Documents\GitHub\NovaGo\Documents\Documents sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FF6480C-09B2-47D6-8296-F72C53E8E128}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94316F6-09F1-490B-9262-4B00C2AB63A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="139">
   <si>
     <t>Nom</t>
   </si>
@@ -454,6 +454,9 @@
   </si>
   <si>
     <t>AJAX déconnexion</t>
+  </si>
+  <si>
+    <t>Stockage sessions dans la BD</t>
   </si>
 </sst>
 </file>
@@ -932,8 +935,8 @@
   </sheetPr>
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1051,7 +1054,9 @@
       <c r="H5" s="7">
         <v>9.5</v>
       </c>
-      <c r="I5" s="7"/>
+      <c r="I5" s="7">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
@@ -1111,7 +1116,7 @@
         <v>7</v>
       </c>
       <c r="H9" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I9" s="7"/>
     </row>
@@ -1164,7 +1169,9 @@
       <c r="G11" s="7">
         <v>7</v>
       </c>
-      <c r="H11" s="7"/>
+      <c r="H11" s="7">
+        <v>7</v>
+      </c>
       <c r="I11" s="7"/>
     </row>
     <row r="12" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1923,8 +1930,8 @@
   </sheetPr>
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2022,6 +2029,12 @@
       <c r="N2" s="17" t="s">
         <v>101</v>
       </c>
+      <c r="O2" s="17">
+        <v>4</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="3" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A3" s="14">
@@ -2066,6 +2079,8 @@
       <c r="N3" s="17" t="s">
         <v>117</v>
       </c>
+      <c r="O3" s="17"/>
+      <c r="P3" s="17"/>
     </row>
     <row r="4" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A4" s="17">
@@ -2106,6 +2121,8 @@
       <c r="N4" s="17" t="s">
         <v>118</v>
       </c>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
     </row>
     <row r="5" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="17">

</xml_diff>

<commit_message>
Fix date_retour post page d'accueil
</commit_message>
<xml_diff>
--- a/Documents/Documents sprint/Feuille_de_temps.xlsx
+++ b/Documents/Documents sprint/Feuille_de_temps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\2034730\Documents\GitHub\NovaGo\Documents\Documents sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40DC344D-17BE-401F-9D8A-62825D50A96A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A564BE4-38C5-41E3-B822-DA136D0E5153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="143">
   <si>
     <t>Nom</t>
   </si>
@@ -466,6 +466,9 @@
   </si>
   <si>
     <t>Stockage sessions dans la BD</t>
+  </si>
+  <si>
+    <t>Déconnexion avec vérification</t>
   </si>
 </sst>
 </file>
@@ -944,8 +947,8 @@
   </sheetPr>
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1064,7 +1067,7 @@
         <v>9.5</v>
       </c>
       <c r="I5" s="7">
-        <v>4</v>
+        <v>5.5</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1963,8 +1966,8 @@
   </sheetPr>
   <dimension ref="A1:P1000"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2063,7 +2066,7 @@
         <v>101</v>
       </c>
       <c r="O2" s="17">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P2" s="17" t="s">
         <v>141</v>
@@ -2111,6 +2114,12 @@
       </c>
       <c r="N3" s="17" t="s">
         <v>117</v>
+      </c>
+      <c r="O3" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="P3" s="17" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
@@ -2152,6 +2161,8 @@
       <c r="N4" s="17" t="s">
         <v>118</v>
       </c>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17"/>
     </row>
     <row r="5" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A5" s="17">

</xml_diff>

<commit_message>
Atelier de français sur la feuille de temps
</commit_message>
<xml_diff>
--- a/Documents/Documents sprint/Feuille_de_temps.xlsx
+++ b/Documents/Documents sprint/Feuille_de_temps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\2034730\Documents\GitHub\NovaGo\Documents\Documents sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F61036-202B-4F59-98FC-E9AD8114349E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E26F004F-1DC6-4532-B8DA-B4881864CCE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="145">
   <si>
     <t>Nom</t>
   </si>
@@ -472,6 +472,9 @@
   </si>
   <si>
     <t>AJAX page connexion</t>
+  </si>
+  <si>
+    <t>Atelier de français</t>
   </si>
 </sst>
 </file>
@@ -951,7 +954,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1015,7 +1018,9 @@
       <c r="H3" s="7">
         <v>11</v>
       </c>
-      <c r="I3" s="7"/>
+      <c r="I3" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
@@ -1042,7 +1047,9 @@
       <c r="H4" s="10">
         <v>9</v>
       </c>
-      <c r="I4" s="10"/>
+      <c r="I4" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -1070,7 +1077,7 @@
         <v>9.5</v>
       </c>
       <c r="I5" s="7">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.25">
@@ -1098,7 +1105,9 @@
       <c r="H6" s="10">
         <v>3</v>
       </c>
-      <c r="I6" s="10"/>
+      <c r="I6" s="10">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -1230,7 +1239,7 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="O4" sqref="O4:P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1434,6 +1443,12 @@
       <c r="N4" t="s">
         <v>123</v>
       </c>
+      <c r="O4" s="17">
+        <v>1</v>
+      </c>
+      <c r="P4" s="17" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15"/>
@@ -1651,7 +1666,7 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="O3" sqref="O3:P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1801,6 +1816,12 @@
       <c r="L3" t="s">
         <v>92</v>
       </c>
+      <c r="O3" s="17">
+        <v>1</v>
+      </c>
+      <c r="P3" s="17" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
@@ -1970,7 +1991,7 @@
   <dimension ref="A1:P1000"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+      <selection activeCell="P5" sqref="O5:P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2210,8 +2231,12 @@
       <c r="N5" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
+      <c r="O5" s="17">
+        <v>1</v>
+      </c>
+      <c r="P5" s="17" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="6" spans="1:16" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17">
@@ -9314,10 +9339,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+      <selection activeCell="O2" sqref="O2:P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9326,7 +9351,7 @@
     <col min="4" max="4" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -9370,7 +9395,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>3</v>
       </c>
@@ -9413,8 +9438,14 @@
       <c r="N2" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="O2" s="17">
+        <v>1</v>
+      </c>
+      <c r="P2" s="17" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -9454,7 +9485,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4">

</xml_diff>

<commit_message>
mise à jour feuille de temps
</commit_message>
<xml_diff>
--- a/Documents/Documents sprint/Feuille_de_temps.xlsx
+++ b/Documents/Documents sprint/Feuille_de_temps.xlsx
@@ -659,10 +659,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9334,7 +9330,7 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="O5" sqref="O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Connexion ajax, regex, redirect v1
</commit_message>
<xml_diff>
--- a/Documents/Documents sprint/Feuille_de_temps.xlsx
+++ b/Documents/Documents sprint/Feuille_de_temps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\NovaGo\Documents\Documents sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941704B5-83E2-4DF9-A307-A1B3C8460E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{000D6042-82AB-4137-92F8-E468CE328A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="158">
   <si>
     <t>Nom</t>
   </si>
@@ -507,7 +507,13 @@
     <t>Formattage page admin (alignement bouton)</t>
   </si>
   <si>
-    <t>AJAX + regex connexion</t>
+    <t>AJAX connexion</t>
+  </si>
+  <si>
+    <t>regex connexion</t>
+  </si>
+  <si>
+    <t>redirect connexion</t>
   </si>
 </sst>
 </file>
@@ -987,8 +993,8 @@
   </sheetPr>
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1121,7 +1127,7 @@
         <v>9</v>
       </c>
       <c r="J5" s="7">
-        <v>4</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
@@ -2078,8 +2084,8 @@
   </sheetPr>
   <dimension ref="A1:R1000"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2190,7 +2196,7 @@
         <v>141</v>
       </c>
       <c r="Q2" s="17">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R2" s="17" t="s">
         <v>155</v>
@@ -2245,8 +2251,12 @@
       <c r="P3" s="17" t="s">
         <v>142</v>
       </c>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
+      <c r="Q3" s="17">
+        <v>1</v>
+      </c>
+      <c r="R3" s="17" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="4" spans="1:18" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A4" s="17">
@@ -2293,8 +2303,12 @@
       <c r="P4" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
+      <c r="Q4" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="R4" s="17" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="5" spans="1:18" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A5" s="17">

</xml_diff>

<commit_message>
Gestion documents de sprint
</commit_message>
<xml_diff>
--- a/Documents/Documents sprint/Feuille_de_temps.xlsx
+++ b/Documents/Documents sprint/Feuille_de_temps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\2034730\Documents\GitHub\NovaGo\Documents\Documents sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCC98BF-3318-431A-AFCB-1702D6D9BF75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{346D6EAA-1AB8-46D4-BC61-35DC5ABC67E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="161">
   <si>
     <t>Nom</t>
   </si>
@@ -520,6 +520,9 @@
   </si>
   <si>
     <t>Faire lettre dans Code nom pour panier</t>
+  </si>
+  <si>
+    <t>Gestion documents</t>
   </si>
 </sst>
 </file>
@@ -2103,7 +2106,7 @@
   <dimension ref="A1:R1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="R5" sqref="R5"/>
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2373,8 +2376,12 @@
       <c r="P5" s="17" t="s">
         <v>148</v>
       </c>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
+      <c r="Q5" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="R5" s="17" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="6" spans="1:18" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="17">

</xml_diff>

<commit_message>
Ajout de plus de redirects
</commit_message>
<xml_diff>
--- a/Documents/Documents sprint/Feuille_de_temps.xlsx
+++ b/Documents/Documents sprint/Feuille_de_temps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\NovaGo\Documents\Documents sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76EAA85-69ED-4CD2-B57F-72876D212029}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD2F39B-DD9B-4626-82B8-A777ADA44148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1012,7 +1012,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1145,7 +1145,7 @@
         <v>9</v>
       </c>
       <c r="J5" s="7">
-        <v>8</v>
+        <v>8.5</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="14.5" x14ac:dyDescent="0.35">
@@ -2127,7 +2127,7 @@
   <dimension ref="A1:R1000"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+      <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2442,7 +2442,7 @@
       <c r="O6" s="17"/>
       <c r="P6" s="17"/>
       <c r="Q6" s="17">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="R6" s="17" t="s">
         <v>161</v>

</xml_diff>

<commit_message>
AJAX, regex, redirect inscription v2
</commit_message>
<xml_diff>
--- a/Documents/Documents sprint/Feuille_de_temps.xlsx
+++ b/Documents/Documents sprint/Feuille_de_temps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\2034730\Documents\GitHub\NovaGo\Documents\Documents sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C9E344-63E5-4021-9568-7990DAECD513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C32C8707-1982-4255-99DA-110224305250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="172">
   <si>
     <t>Nom</t>
   </si>
@@ -553,6 +553,9 @@
   </si>
   <si>
     <t>Affichage séparé des erreurs AJAX de connexion</t>
+  </si>
+  <si>
+    <t>AJAX regex redirect du post d'inscription</t>
   </si>
 </sst>
 </file>
@@ -1033,7 +1036,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1195,7 +1198,7 @@
         <v>9</v>
       </c>
       <c r="K5" s="7">
-        <v>0.5</v>
+        <v>4</v>
       </c>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
@@ -2288,7 +2291,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="T4" sqref="T4"/>
+      <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2624,8 +2627,12 @@
       <c r="R5" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="S5" s="15"/>
-      <c r="T5" s="17"/>
+      <c r="S5" s="15">
+        <v>2</v>
+      </c>
+      <c r="T5" s="17" t="s">
+        <v>171</v>
+      </c>
       <c r="U5" s="15"/>
       <c r="V5" s="15"/>
       <c r="W5" s="15"/>

</xml_diff>

<commit_message>
feuille de temps billy
</commit_message>
<xml_diff>
--- a/Documents/Documents sprint/Feuille_de_temps.xlsx
+++ b/Documents/Documents sprint/Feuille_de_temps.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\AWT\NovaGo\Documents\Documents sprint\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lechu\Documents\GitHub\NovaGo\Documents\Documents sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED09432D-5B9E-48C2-A7DD-2FFF17E91E27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C40363-D828-42E6-8746-FE21FCBAC4A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4905" yWindow="990" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sommaire" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="178">
   <si>
     <t>Nom</t>
   </si>
@@ -562,6 +562,18 @@
   </si>
   <si>
     <t>Désamorçage du dépôt github</t>
+  </si>
+  <si>
+    <t>Connecter Recherche à Reservation</t>
+  </si>
+  <si>
+    <t>Connecter Stripe à Reservation</t>
+  </si>
+  <si>
+    <t>Fix Github</t>
+  </si>
+  <si>
+    <t>Fix Reservation JS -&gt; mini erreur</t>
   </si>
 </sst>
 </file>
@@ -740,7 +752,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1045,7 +1057,7 @@
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
@@ -1411,11 +1423,11 @@
   </sheetPr>
   <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
       <selection activeCell="S3" sqref="S3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="36.140625" customWidth="1"/>
     <col min="4" max="4" width="26.5703125" customWidth="1"/>
@@ -1425,6 +1437,8 @@
     <col min="10" max="10" width="36.42578125" customWidth="1"/>
     <col min="12" max="12" width="30.5703125" customWidth="1"/>
     <col min="14" max="14" width="57" customWidth="1"/>
+    <col min="18" max="18" width="36.28515625" customWidth="1"/>
+    <col min="20" max="20" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15" x14ac:dyDescent="0.25">
@@ -1624,6 +1638,12 @@
       <c r="R3" t="s">
         <v>159</v>
       </c>
+      <c r="S3">
+        <v>2</v>
+      </c>
+      <c r="T3" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="4" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15">
@@ -1675,6 +1695,12 @@
       </c>
       <c r="R4" t="s">
         <v>161</v>
+      </c>
+      <c r="S4">
+        <v>2</v>
+      </c>
+      <c r="T4" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1724,6 +1750,12 @@
       <c r="R5" t="s">
         <v>158</v>
       </c>
+      <c r="S5">
+        <v>1</v>
+      </c>
+      <c r="T5" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15"/>
@@ -1759,6 +1791,12 @@
       </c>
       <c r="N6" t="s">
         <v>126</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1904,11 +1942,11 @@
   </sheetPr>
   <dimension ref="A1:Z15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+    <sheetView topLeftCell="O1" workbookViewId="0">
       <selection activeCell="T9" sqref="T9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="21.5703125" customWidth="1"/>
     <col min="8" max="8" width="33.5703125" customWidth="1"/>
@@ -2312,7 +2350,7 @@
       <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:26" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -9787,7 +9825,7 @@
       <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
     <col min="4" max="4" width="32" customWidth="1"/>

</xml_diff>

<commit_message>
Removed les locals + validation visuelle sur inscription
</commit_message>
<xml_diff>
--- a/Documents/Documents sprint/Feuille_de_temps.xlsx
+++ b/Documents/Documents sprint/Feuille_de_temps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\2034730\Documents\GitHub\NovaGo\Documents\Documents sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417C86DD-6B71-4EF6-9084-6A512DF2CD72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6893EA8-265F-4F4D-91BD-72DE8FA66AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="184">
   <si>
     <t>Nom</t>
   </si>
@@ -583,6 +583,15 @@
   </si>
   <si>
     <t>Mongo DB</t>
+  </si>
+  <si>
+    <t>Répartition tâches</t>
+  </si>
+  <si>
+    <t>Fix double connexion</t>
+  </si>
+  <si>
+    <t>Affichages visuels champs erreur</t>
   </si>
 </sst>
 </file>
@@ -1063,7 +1072,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1187,7 +1196,7 @@
         <v>11</v>
       </c>
       <c r="K4" s="10">
-        <v>0.5</v>
+        <v>6.5</v>
       </c>
       <c r="L4" s="10"/>
       <c r="M4" s="10"/>
@@ -1227,7 +1236,9 @@
       <c r="K5" s="7">
         <v>7</v>
       </c>
-      <c r="L5" s="7"/>
+      <c r="L5" s="7">
+        <v>4</v>
+      </c>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
     </row>
@@ -1262,7 +1273,9 @@
       <c r="J6" s="10">
         <v>3</v>
       </c>
-      <c r="K6" s="10"/>
+      <c r="K6" s="10">
+        <v>2</v>
+      </c>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
@@ -1306,7 +1319,9 @@
       <c r="J9" s="7">
         <v>7</v>
       </c>
-      <c r="K9" s="7"/>
+      <c r="K9" s="7">
+        <v>7</v>
+      </c>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
@@ -1342,7 +1357,9 @@
       <c r="J10" s="10">
         <v>8</v>
       </c>
-      <c r="K10" s="10"/>
+      <c r="K10" s="10">
+        <v>6</v>
+      </c>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
@@ -1378,7 +1395,9 @@
       <c r="J11" s="7">
         <v>7</v>
       </c>
-      <c r="K11" s="7"/>
+      <c r="K11" s="7">
+        <v>7</v>
+      </c>
       <c r="L11" s="7"/>
       <c r="M11" s="7"/>
       <c r="N11" s="7"/>
@@ -1414,7 +1433,9 @@
       <c r="J12" s="10">
         <v>3</v>
       </c>
-      <c r="K12" s="10"/>
+      <c r="K12" s="10">
+        <v>0</v>
+      </c>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
       <c r="N12" s="10"/>
@@ -1433,7 +1454,7 @@
   <dimension ref="A1:Z15"/>
   <sheetViews>
     <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+      <selection activeCell="T7" sqref="T7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2362,7 +2383,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="U6" sqref="U6"/>
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2508,8 +2529,12 @@
       <c r="T2" s="17" t="s">
         <v>160</v>
       </c>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
+      <c r="U2" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="V2" s="17" t="s">
+        <v>181</v>
+      </c>
       <c r="W2" s="15"/>
       <c r="X2" s="15"/>
       <c r="Y2" s="15"/>
@@ -2576,8 +2601,12 @@
       <c r="T3" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="U3" s="15"/>
-      <c r="V3" s="15"/>
+      <c r="U3" s="15">
+        <v>1</v>
+      </c>
+      <c r="V3" s="17" t="s">
+        <v>182</v>
+      </c>
       <c r="W3" s="15"/>
       <c r="X3" s="15"/>
       <c r="Y3" s="15"/>
@@ -2640,8 +2669,12 @@
       <c r="T4" s="17" t="s">
         <v>170</v>
       </c>
-      <c r="U4" s="15"/>
-      <c r="V4" s="15"/>
+      <c r="U4" s="15">
+        <v>2.5</v>
+      </c>
+      <c r="V4" s="17" t="s">
+        <v>183</v>
+      </c>
       <c r="W4" s="15"/>
       <c r="X4" s="15"/>
       <c r="Y4" s="15"/>

</xml_diff>

<commit_message>
Fix affichage des messages page index
</commit_message>
<xml_diff>
--- a/Documents/Documents sprint/Feuille_de_temps.xlsx
+++ b/Documents/Documents sprint/Feuille_de_temps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\NovaGo\Documents\Documents sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D789AA62-2289-4850-AAD0-5910AE449D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42348BD4-6A71-4DB9-8877-0C4FD2969FD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -624,7 +624,7 @@
     <t>Regex index</t>
   </si>
   <si>
-    <t>Fix post index</t>
+    <t>Fix post/affichage index</t>
   </si>
 </sst>
 </file>
@@ -2461,7 +2461,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+      <selection activeCell="V3" sqref="V3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2610,7 +2610,7 @@
       <c r="U2" s="15">
         <v>0.5</v>
       </c>
-      <c r="V2" s="15" t="s">
+      <c r="V2" s="17" t="s">
         <v>184</v>
       </c>
       <c r="W2" s="15"/>
@@ -2682,7 +2682,7 @@
       <c r="U3" s="15">
         <v>1</v>
       </c>
-      <c r="V3" s="15" t="s">
+      <c r="V3" s="17" t="s">
         <v>185</v>
       </c>
       <c r="W3" s="15"/>
@@ -2750,7 +2750,7 @@
       <c r="U4" s="15">
         <v>2.5</v>
       </c>
-      <c r="V4" s="15" t="s">
+      <c r="V4" s="17" t="s">
         <v>186</v>
       </c>
       <c r="W4" s="15"/>
@@ -2818,7 +2818,7 @@
       <c r="U5" s="15">
         <v>1.5</v>
       </c>
-      <c r="V5" s="15" t="s">
+      <c r="V5" s="17" t="s">
         <v>191</v>
       </c>
       <c r="W5" s="15"/>
@@ -2878,7 +2878,7 @@
       <c r="U6" s="15">
         <v>0.5</v>
       </c>
-      <c r="V6" s="15" t="s">
+      <c r="V6" s="17" t="s">
         <v>192</v>
       </c>
       <c r="W6" s="15"/>
@@ -2928,7 +2928,7 @@
       <c r="U7" s="15">
         <v>2.5</v>
       </c>
-      <c r="V7" s="15" t="s">
+      <c r="V7" s="17" t="s">
         <v>193</v>
       </c>
       <c r="W7" s="15"/>
@@ -2964,7 +2964,7 @@
       <c r="U8" s="15">
         <v>0.5</v>
       </c>
-      <c r="V8" s="15" t="s">
+      <c r="V8" s="17" t="s">
         <v>194</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix post index admin
</commit_message>
<xml_diff>
--- a/Documents/Documents sprint/Feuille_de_temps.xlsx
+++ b/Documents/Documents sprint/Feuille_de_temps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\2034730\Documents\GitHub\NovaGo\Documents\Documents sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD72DA22-FA48-4DA0-8A3C-DE88A1716BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92E52104-2F5F-4C46-8EAB-D91E77F5714C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="203">
   <si>
     <t>Nom</t>
   </si>
@@ -637,6 +637,18 @@
   </si>
   <si>
     <t>Gestion session (locals) pour stocker l'info d'index</t>
+  </si>
+  <si>
+    <t>Lecture des commentaires de mongoDB</t>
+  </si>
+  <si>
+    <t>Modifications navbar</t>
+  </si>
+  <si>
+    <t>Post index verification deplacement</t>
+  </si>
+  <si>
+    <t>Fix + ajouts affichage page reservation</t>
   </si>
 </sst>
 </file>
@@ -1120,7 +1132,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1291,7 +1303,9 @@
       <c r="L5" s="7">
         <v>9</v>
       </c>
-      <c r="M5" s="7"/>
+      <c r="M5" s="7">
+        <v>7.5</v>
+      </c>
       <c r="N5" s="7"/>
     </row>
     <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.25">
@@ -2495,7 +2509,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="U6" sqref="U6"/>
+      <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2648,7 +2662,7 @@
         <v>184</v>
       </c>
       <c r="W2" s="15">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="X2" s="17" t="s">
         <v>196</v>
@@ -2867,8 +2881,12 @@
       <c r="V5" s="17" t="s">
         <v>191</v>
       </c>
-      <c r="W5" s="15"/>
-      <c r="X5" s="17"/>
+      <c r="W5" s="15">
+        <v>2</v>
+      </c>
+      <c r="X5" s="17" t="s">
+        <v>199</v>
+      </c>
       <c r="Y5" s="15"/>
       <c r="Z5" s="15"/>
     </row>
@@ -2927,8 +2945,12 @@
       <c r="V6" s="17" t="s">
         <v>192</v>
       </c>
-      <c r="W6" s="15"/>
-      <c r="X6" s="17"/>
+      <c r="W6" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="X6" s="17" t="s">
+        <v>200</v>
+      </c>
       <c r="Y6" s="15"/>
       <c r="Z6" s="15"/>
     </row>
@@ -2977,8 +2999,12 @@
       <c r="V7" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="W7" s="15"/>
-      <c r="X7" s="17"/>
+      <c r="W7" s="15">
+        <v>0.5</v>
+      </c>
+      <c r="X7" s="17" t="s">
+        <v>201</v>
+      </c>
       <c r="Y7" s="15"/>
       <c r="Z7" s="15"/>
     </row>
@@ -3013,7 +3039,12 @@
       <c r="V8" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="X8" s="21"/>
+      <c r="W8" s="15">
+        <v>1</v>
+      </c>
+      <c r="X8" s="21" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="12"/>

</xml_diff>